<commit_message>
merged new changes for PEEK model in SAFT-g Mie and updated PVT data for PEEK .
</commit_message>
<xml_diff>
--- a/litdata/CO2-PS.xlsx
+++ b/litdata/CO2-PS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B4F71B9-7966-47A1-BA83-CDF282995EFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{453BD694-E4E0-405A-925C-1EC2D35ED005}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="32" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="42" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!S_25C_1.049" sheetId="7" state="hidden" r:id="rId1"/>
@@ -50,10 +50,10 @@
     <sheet name="S_35C (23)" sheetId="34" r:id="rId40"/>
     <sheet name="S_80C (24)" sheetId="38" r:id="rId41"/>
     <sheet name="!S_25C (25)" sheetId="39" r:id="rId42"/>
-    <sheet name="S_65C (26)" sheetId="41" r:id="rId43"/>
-    <sheet name="S_90C (26)" sheetId="42" r:id="rId44"/>
-    <sheet name="S_110C (26)" sheetId="45" r:id="rId45"/>
-    <sheet name="S_130C (26)" sheetId="44" r:id="rId46"/>
+    <sheet name="!S_65C (26)" sheetId="41" r:id="rId43"/>
+    <sheet name="!S_90C (26)" sheetId="42" r:id="rId44"/>
+    <sheet name="!S_110C (26)" sheetId="45" r:id="rId45"/>
+    <sheet name="!S_130C (26)" sheetId="44" r:id="rId46"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="89">
   <si>
     <t>P [MPa]</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>_fit_ksw_NE?_</t>
+  </si>
+  <si>
+    <t>Same as Hilic 2001 (20)</t>
   </si>
 </sst>
 </file>
@@ -7164,7 +7167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B958F3-9747-43D3-B52B-6645775C2715}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -13483,7 +13486,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13569,8 +13572,8 @@
       <c r="D4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>74</v>
+      <c r="F4" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="G4"/>
     </row>
@@ -13645,7 +13648,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13725,8 +13728,8 @@
       <c r="D4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>74</v>
+      <c r="G4" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -13815,7 +13818,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13895,8 +13898,8 @@
       <c r="D4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>74</v>
+      <c r="G4" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -14029,8 +14032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1A4BA1-A803-46D7-8AF8-568D2FEFE7FD}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14110,8 +14113,8 @@
       <c r="D4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>74</v>
+      <c r="G4" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>